<commit_message>
Backup before implementing stiffening feature
</commit_message>
<xml_diff>
--- a/Final_Design/WingBoxAnalysis_v2/NACA0012_Points.xlsx
+++ b/Final_Design/WingBoxAnalysis_v2/NACA0012_Points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/273b60a69ebe275f/Desktop/SMM/Final_Design/WingBox_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/273b60a69ebe275f/Desktop/SMM/Final_Design/WingBoxAnalysis_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{471818F7-BB20-40A4-97AF-4CD4727E7021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{471818F7-BB20-40A4-97AF-4CD4727E7021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8B194D08-3BDF-4A2D-8BA5-31B00EC7C5C2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,19 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,277 +389,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>0</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>5.8390000000000004E-4</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>4.2602999999999999E-3</v>
+        <v>1.2600000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2.3341999999999998E-3</v>
+        <v>0.99941610000000003</v>
       </c>
       <c r="B3">
-        <v>8.4288999999999996E-3</v>
+        <v>1.3419E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>5.2468000000000002E-3</v>
+        <v>0.99766580000000005</v>
       </c>
       <c r="B4">
-        <v>1.2501099999999999E-2</v>
+        <v>1.5870000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>9.3148999999999992E-3</v>
+        <v>0.9947532</v>
       </c>
       <c r="B5">
-        <v>1.6470599999999998E-2</v>
+        <v>1.9938E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1.45291E-2</v>
+        <v>0.99068500000000004</v>
       </c>
       <c r="B6">
-        <v>2.0330000000000001E-2</v>
+        <v>2.5595000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2.0877099999999999E-2</v>
+        <v>0.98547090000000004</v>
       </c>
       <c r="B7">
-        <v>2.4070600000000001E-2</v>
+        <v>3.2804000000000002E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2.8344100000000001E-2</v>
+        <v>0.97912290000000002</v>
       </c>
       <c r="B8">
-        <v>2.7682700000000001E-2</v>
+        <v>4.1519E-3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3.69127E-2</v>
+        <v>0.97165590000000002</v>
       </c>
       <c r="B9">
-        <v>3.11559E-2</v>
+        <v>5.1685000000000004E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4.6562800000000001E-2</v>
+        <v>0.96308729999999998</v>
       </c>
       <c r="B10">
-        <v>3.4479200000000002E-2</v>
+        <v>6.3238000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>5.7272000000000003E-2</v>
+        <v>0.95343719999999998</v>
       </c>
       <c r="B11">
-        <v>3.7641399999999998E-2</v>
+        <v>7.6108E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>6.9015199999999999E-2</v>
+        <v>0.94272800000000001</v>
       </c>
       <c r="B12">
-        <v>4.0631E-2</v>
+        <v>9.0217000000000006E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>8.1764900000000001E-2</v>
+        <v>0.9309849</v>
       </c>
       <c r="B13">
-        <v>4.3437099999999999E-2</v>
+        <v>1.0548500000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>9.5491500000000007E-2</v>
+        <v>0.91823509999999997</v>
       </c>
       <c r="B14">
-        <v>4.6048899999999997E-2</v>
+        <v>1.21823E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0.11016280000000001</v>
+        <v>0.90450850000000005</v>
       </c>
       <c r="B15">
-        <v>4.8456699999999998E-2</v>
+        <v>1.3914299999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0.12574460000000001</v>
+        <v>0.88983719999999999</v>
       </c>
       <c r="B16">
-        <v>5.0651300000000003E-2</v>
+        <v>1.5735099999999998E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0.14220050000000001</v>
+        <v>0.87425540000000002</v>
       </c>
       <c r="B17">
-        <v>5.2625100000000001E-2</v>
+        <v>1.76353E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0.1594921</v>
+        <v>0.85779950000000005</v>
       </c>
       <c r="B18">
-        <v>5.4371500000000003E-2</v>
+        <v>1.96051E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0.17757890000000001</v>
+        <v>0.84050789999999997</v>
       </c>
       <c r="B19">
-        <v>5.5885600000000001E-2</v>
+        <v>2.16347E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0.1964187</v>
+        <v>0.82242110000000002</v>
       </c>
       <c r="B20">
-        <v>5.7164E-2</v>
+        <v>2.3714200000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>0.21596760000000001</v>
+        <v>0.80358130000000005</v>
       </c>
       <c r="B21">
-        <v>5.8204800000000001E-2</v>
+        <v>2.5833700000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0.2361799</v>
+        <v>0.78403239999999996</v>
       </c>
       <c r="B22">
-        <v>5.9008100000000001E-2</v>
+        <v>2.7982799999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>0.25700830000000002</v>
+        <v>0.76382019999999995</v>
       </c>
       <c r="B23">
-        <v>5.9575500000000003E-2</v>
+        <v>3.0151500000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>0.27840419999999999</v>
+        <v>0.74299170000000003</v>
       </c>
       <c r="B24">
-        <v>5.9910199999999997E-2</v>
+        <v>3.2329400000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>0.30031770000000002</v>
+        <v>0.72159580000000001</v>
       </c>
       <c r="B25">
-        <v>6.00172E-2</v>
+        <v>3.4505800000000003E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>0.32269759999999997</v>
+        <v>0.69968229999999998</v>
       </c>
       <c r="B26">
-        <v>5.9902799999999999E-2</v>
+        <v>3.6670000000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>0.34549150000000001</v>
+        <v>0.67730250000000003</v>
       </c>
       <c r="B27">
-        <v>5.9574700000000001E-2</v>
+        <v>3.8810900000000002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>0.36864629999999998</v>
+        <v>0.65450850000000005</v>
       </c>
       <c r="B28">
-        <v>5.9041900000000001E-2</v>
+        <v>4.09174E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>0.39210790000000001</v>
+        <v>0.63135370000000002</v>
       </c>
       <c r="B29">
-        <v>5.8314499999999998E-2</v>
+        <v>4.2977799999999997E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0.41582150000000001</v>
+        <v>0.60789210000000005</v>
       </c>
       <c r="B30">
-        <v>5.7403299999999997E-2</v>
+        <v>4.4980199999999998E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0.4397317</v>
+        <v>0.58417859999999999</v>
       </c>
       <c r="B31">
-        <v>5.6320000000000002E-2</v>
+        <v>4.69124E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>0.46378259999999999</v>
+        <v>0.56026830000000005</v>
       </c>
       <c r="B32">
-        <v>5.5076899999999998E-2</v>
+        <v>4.8761899999999997E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>0.48791810000000002</v>
+        <v>0.53621739999999996</v>
       </c>
       <c r="B33">
-        <v>5.3686600000000001E-2</v>
+        <v>5.0516100000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -661,791 +672,791 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>0.53621739999999996</v>
+        <v>0.48791810000000002</v>
       </c>
       <c r="B35">
-        <v>5.0516100000000001E-2</v>
+        <v>5.3686600000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>0.56026830000000005</v>
+        <v>0.46378259999999999</v>
       </c>
       <c r="B36">
-        <v>4.8761899999999997E-2</v>
+        <v>5.5076899999999998E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>0.58417859999999999</v>
+        <v>0.4397317</v>
       </c>
       <c r="B37">
-        <v>4.69124E-2</v>
+        <v>5.6320000000000002E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>0.60789210000000005</v>
+        <v>0.41582150000000001</v>
       </c>
       <c r="B38">
-        <v>4.4980199999999998E-2</v>
+        <v>5.7403299999999997E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>0.63135370000000002</v>
+        <v>0.39210790000000001</v>
       </c>
       <c r="B39">
-        <v>4.2977799999999997E-2</v>
+        <v>5.8314499999999998E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>0.65450850000000005</v>
+        <v>0.36864629999999998</v>
       </c>
       <c r="B40">
-        <v>4.09174E-2</v>
+        <v>5.9041900000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>0.67730250000000003</v>
+        <v>0.34549150000000001</v>
       </c>
       <c r="B41">
-        <v>3.8810900000000002E-2</v>
+        <v>5.9574700000000001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>0.69968229999999998</v>
+        <v>0.32269759999999997</v>
       </c>
       <c r="B42">
-        <v>3.6670000000000001E-2</v>
+        <v>5.9902799999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>0.72159580000000001</v>
+        <v>0.30031770000000002</v>
       </c>
       <c r="B43">
-        <v>3.4505800000000003E-2</v>
+        <v>6.00172E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>0.74299170000000003</v>
+        <v>0.27840419999999999</v>
       </c>
       <c r="B44">
-        <v>3.2329400000000001E-2</v>
+        <v>5.9910199999999997E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>0.76382019999999995</v>
+        <v>0.25700830000000002</v>
       </c>
       <c r="B45">
-        <v>3.0151500000000001E-2</v>
+        <v>5.9575500000000003E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>0.78403239999999996</v>
+        <v>0.2361799</v>
       </c>
       <c r="B46">
-        <v>2.7982799999999999E-2</v>
+        <v>5.9008100000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>0.80358130000000005</v>
+        <v>0.21596760000000001</v>
       </c>
       <c r="B47">
-        <v>2.5833700000000001E-2</v>
+        <v>5.8204800000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>0.82242110000000002</v>
+        <v>0.1964187</v>
       </c>
       <c r="B48">
-        <v>2.3714200000000001E-2</v>
+        <v>5.7164E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>0.84050789999999997</v>
+        <v>0.17757890000000001</v>
       </c>
       <c r="B49">
-        <v>2.16347E-2</v>
+        <v>5.5885600000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>0.85779950000000005</v>
+        <v>0.1594921</v>
       </c>
       <c r="B50">
-        <v>1.96051E-2</v>
+        <v>5.4371500000000003E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>0.87425540000000002</v>
+        <v>0.14220050000000001</v>
       </c>
       <c r="B51">
-        <v>1.76353E-2</v>
+        <v>5.2625100000000001E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>0.88983719999999999</v>
+        <v>0.12574460000000001</v>
       </c>
       <c r="B52">
-        <v>1.5735099999999998E-2</v>
+        <v>5.0651300000000003E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>0.90450850000000005</v>
+        <v>0.11016280000000001</v>
       </c>
       <c r="B53">
-        <v>1.3914299999999999E-2</v>
+        <v>4.8456699999999998E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>0.91823509999999997</v>
+        <v>9.5491500000000007E-2</v>
       </c>
       <c r="B54">
-        <v>1.21823E-2</v>
+        <v>4.6048899999999997E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>0.9309849</v>
+        <v>8.1764900000000001E-2</v>
       </c>
       <c r="B55">
-        <v>1.0548500000000001E-2</v>
+        <v>4.3437099999999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>0.94272800000000001</v>
+        <v>6.9015199999999999E-2</v>
       </c>
       <c r="B56">
-        <v>9.0217000000000006E-3</v>
+        <v>4.0631E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>0.95343719999999998</v>
+        <v>5.7272000000000003E-2</v>
       </c>
       <c r="B57">
-        <v>7.6108E-3</v>
+        <v>3.7641399999999998E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>0.96308729999999998</v>
+        <v>4.6562800000000001E-2</v>
       </c>
       <c r="B58">
-        <v>6.3238000000000001E-3</v>
+        <v>3.4479200000000002E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>0.97165590000000002</v>
+        <v>3.69127E-2</v>
       </c>
       <c r="B59">
-        <v>5.1685000000000004E-3</v>
+        <v>3.11559E-2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>0.97912290000000002</v>
+        <v>2.8344100000000001E-2</v>
       </c>
       <c r="B60">
-        <v>4.1519E-3</v>
+        <v>2.7682700000000001E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>0.98547090000000004</v>
+        <v>2.0877099999999999E-2</v>
       </c>
       <c r="B61">
-        <v>3.2804000000000002E-3</v>
+        <v>2.4070600000000001E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>0.99068500000000004</v>
+        <v>1.45291E-2</v>
       </c>
       <c r="B62">
-        <v>2.5595000000000001E-3</v>
+        <v>2.0330000000000001E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>0.9947532</v>
+        <v>9.3148999999999992E-3</v>
       </c>
       <c r="B63">
-        <v>1.9938E-3</v>
+        <v>1.6470599999999998E-2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>0.99766580000000005</v>
+        <v>5.2468000000000002E-3</v>
       </c>
       <c r="B64">
-        <v>1.5870000000000001E-3</v>
+        <v>1.2501099999999999E-2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>0.99941610000000003</v>
+        <v>2.3341999999999998E-3</v>
       </c>
       <c r="B65">
-        <v>1.3419E-3</v>
+        <v>8.4288999999999996E-3</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>1</v>
+        <v>5.8390000000000004E-4</v>
       </c>
       <c r="B66">
-        <v>1.2600000000000001E-3</v>
+        <v>4.2602999999999999E-3</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B67">
-        <v>-1.2600000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>0.99941610000000003</v>
+        <v>5.8390000000000004E-4</v>
       </c>
       <c r="B68">
-        <v>-1.3419E-3</v>
+        <v>-4.2602999999999999E-3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>0.99766580000000005</v>
+        <v>2.3341999999999998E-3</v>
       </c>
       <c r="B69">
-        <v>-1.5870000000000001E-3</v>
+        <v>-8.4288999999999996E-3</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>0.9947532</v>
+        <v>5.2468000000000002E-3</v>
       </c>
       <c r="B70">
-        <v>-1.9938E-3</v>
+        <v>-1.2501099999999999E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>0.99068500000000004</v>
+        <v>9.3148999999999992E-3</v>
       </c>
       <c r="B71">
-        <v>-2.5595000000000001E-3</v>
+        <v>-1.6470599999999998E-2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>0.98547090000000004</v>
+        <v>1.45291E-2</v>
       </c>
       <c r="B72">
-        <v>-3.2804000000000002E-3</v>
+        <v>-2.0330000000000001E-2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>0.97912290000000002</v>
+        <v>2.0877099999999999E-2</v>
       </c>
       <c r="B73">
-        <v>-4.1519E-3</v>
+        <v>-2.4070600000000001E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>0.97165590000000002</v>
+        <v>2.8344100000000001E-2</v>
       </c>
       <c r="B74">
-        <v>-5.1685000000000004E-3</v>
+        <v>-2.7682700000000001E-2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>0.96308729999999998</v>
+        <v>3.69127E-2</v>
       </c>
       <c r="B75">
-        <v>-6.3238000000000001E-3</v>
+        <v>-3.11559E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>0.95343719999999998</v>
+        <v>4.6562800000000001E-2</v>
       </c>
       <c r="B76">
-        <v>-7.6108E-3</v>
+        <v>-3.4479200000000002E-2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>0.94272800000000001</v>
+        <v>5.7272000000000003E-2</v>
       </c>
       <c r="B77">
-        <v>-9.0217000000000006E-3</v>
+        <v>-3.7641399999999998E-2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>0.9309849</v>
+        <v>6.9015199999999999E-2</v>
       </c>
       <c r="B78">
-        <v>-1.0548500000000001E-2</v>
+        <v>-4.0631E-2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>0.91823509999999997</v>
+        <v>8.1764900000000001E-2</v>
       </c>
       <c r="B79">
-        <v>-1.21823E-2</v>
+        <v>-4.3437099999999999E-2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>0.90450850000000005</v>
+        <v>9.5491500000000007E-2</v>
       </c>
       <c r="B80">
-        <v>-1.3914299999999999E-2</v>
+        <v>-4.6048899999999997E-2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>0.88983719999999999</v>
+        <v>0.11016280000000001</v>
       </c>
       <c r="B81">
-        <v>-1.5735099999999998E-2</v>
+        <v>-4.8456699999999998E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>0.87425540000000002</v>
+        <v>0.12574460000000001</v>
       </c>
       <c r="B82">
-        <v>-1.76353E-2</v>
+        <v>-5.0651300000000003E-2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>0.85779950000000005</v>
+        <v>0.14220050000000001</v>
       </c>
       <c r="B83">
-        <v>-1.96051E-2</v>
+        <v>-5.2625100000000001E-2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>0.84050789999999997</v>
+        <v>0.1594921</v>
       </c>
       <c r="B84">
-        <v>-2.16347E-2</v>
+        <v>-5.4371500000000003E-2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>0.82242110000000002</v>
+        <v>0.17757890000000001</v>
       </c>
       <c r="B85">
-        <v>-2.3714200000000001E-2</v>
+        <v>-5.5885600000000001E-2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>0.80358130000000005</v>
+        <v>0.1964187</v>
       </c>
       <c r="B86">
-        <v>-2.5833700000000001E-2</v>
+        <v>-5.7164E-2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>0.78403239999999996</v>
+        <v>0.21596760000000001</v>
       </c>
       <c r="B87">
-        <v>-2.7982799999999999E-2</v>
+        <v>-5.8204800000000001E-2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>0.76382019999999995</v>
+        <v>0.2361799</v>
       </c>
       <c r="B88">
-        <v>-3.0151500000000001E-2</v>
+        <v>-5.9008100000000001E-2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>0.74299170000000003</v>
+        <v>0.25700830000000002</v>
       </c>
       <c r="B89">
-        <v>-3.2329400000000001E-2</v>
+        <v>-5.9575500000000003E-2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>0.72159580000000001</v>
+        <v>0.27840419999999999</v>
       </c>
       <c r="B90">
-        <v>-3.4505800000000003E-2</v>
+        <v>-5.9910199999999997E-2</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>0.69968229999999998</v>
+        <v>0.30031770000000002</v>
       </c>
       <c r="B91">
-        <v>-3.6670000000000001E-2</v>
+        <v>-6.00172E-2</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>0.67730250000000003</v>
+        <v>0.32269759999999997</v>
       </c>
       <c r="B92">
-        <v>-3.8810900000000002E-2</v>
+        <v>-5.9902799999999999E-2</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>0.65450850000000005</v>
+        <v>0.34549150000000001</v>
       </c>
       <c r="B93">
-        <v>-4.09174E-2</v>
+        <v>-5.9574700000000001E-2</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>0.63135370000000002</v>
+        <v>0.36864629999999998</v>
       </c>
       <c r="B94">
-        <v>-4.2977799999999997E-2</v>
+        <v>-5.9041900000000001E-2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>0.60789210000000005</v>
+        <v>0.39210790000000001</v>
       </c>
       <c r="B95">
-        <v>-4.4980199999999998E-2</v>
+        <v>-5.8314499999999998E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>0.58417859999999999</v>
+        <v>0.41582150000000001</v>
       </c>
       <c r="B96">
-        <v>-4.69124E-2</v>
+        <v>-5.7403299999999997E-2</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>0.56026830000000005</v>
+        <v>0.4397317</v>
       </c>
       <c r="B97">
-        <v>-4.8761899999999997E-2</v>
+        <v>-5.6320000000000002E-2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>0.53621739999999996</v>
+        <v>0.46378259999999999</v>
       </c>
       <c r="B98">
-        <v>-5.0516100000000001E-2</v>
+        <v>-5.5076899999999998E-2</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>0.51208189999999998</v>
+        <v>0.48791810000000002</v>
       </c>
       <c r="B99">
-        <v>-5.2162E-2</v>
+        <v>-5.3686600000000001E-2</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>0.48791810000000002</v>
+        <v>0.51208189999999998</v>
       </c>
       <c r="B100">
-        <v>-5.3686600000000001E-2</v>
+        <v>-5.2162E-2</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>0.46378259999999999</v>
+        <v>0.53621739999999996</v>
       </c>
       <c r="B101">
-        <v>-5.5076899999999998E-2</v>
+        <v>-5.0516100000000001E-2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>0.4397317</v>
+        <v>0.56026830000000005</v>
       </c>
       <c r="B102">
-        <v>-5.6320000000000002E-2</v>
+        <v>-4.8761899999999997E-2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>0.41582150000000001</v>
+        <v>0.58417859999999999</v>
       </c>
       <c r="B103">
-        <v>-5.7403299999999997E-2</v>
+        <v>-4.69124E-2</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>0.39210790000000001</v>
+        <v>0.60789210000000005</v>
       </c>
       <c r="B104">
-        <v>-5.8314499999999998E-2</v>
+        <v>-4.4980199999999998E-2</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>0.36864629999999998</v>
+        <v>0.63135370000000002</v>
       </c>
       <c r="B105">
-        <v>-5.9041900000000001E-2</v>
+        <v>-4.2977799999999997E-2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>0.34549150000000001</v>
+        <v>0.65450850000000005</v>
       </c>
       <c r="B106">
-        <v>-5.9574700000000001E-2</v>
+        <v>-4.09174E-2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>0.32269759999999997</v>
+        <v>0.67730250000000003</v>
       </c>
       <c r="B107">
-        <v>-5.9902799999999999E-2</v>
+        <v>-3.8810900000000002E-2</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>0.30031770000000002</v>
+        <v>0.69968229999999998</v>
       </c>
       <c r="B108">
-        <v>-6.00172E-2</v>
+        <v>-3.6670000000000001E-2</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>0.27840419999999999</v>
+        <v>0.72159580000000001</v>
       </c>
       <c r="B109">
-        <v>-5.9910199999999997E-2</v>
+        <v>-3.4505800000000003E-2</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>0.25700830000000002</v>
+        <v>0.74299170000000003</v>
       </c>
       <c r="B110">
-        <v>-5.9575500000000003E-2</v>
+        <v>-3.2329400000000001E-2</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>0.2361799</v>
+        <v>0.76382019999999995</v>
       </c>
       <c r="B111">
-        <v>-5.9008100000000001E-2</v>
+        <v>-3.0151500000000001E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>0.21596760000000001</v>
+        <v>0.78403239999999996</v>
       </c>
       <c r="B112">
-        <v>-5.8204800000000001E-2</v>
+        <v>-2.7982799999999999E-2</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>0.1964187</v>
+        <v>0.80358130000000005</v>
       </c>
       <c r="B113">
-        <v>-5.7164E-2</v>
+        <v>-2.5833700000000001E-2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>0.17757890000000001</v>
+        <v>0.82242110000000002</v>
       </c>
       <c r="B114">
-        <v>-5.5885600000000001E-2</v>
+        <v>-2.3714200000000001E-2</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>0.1594921</v>
+        <v>0.84050789999999997</v>
       </c>
       <c r="B115">
-        <v>-5.4371500000000003E-2</v>
+        <v>-2.16347E-2</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>0.14220050000000001</v>
+        <v>0.85779950000000005</v>
       </c>
       <c r="B116">
-        <v>-5.2625100000000001E-2</v>
+        <v>-1.96051E-2</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>0.12574460000000001</v>
+        <v>0.87425540000000002</v>
       </c>
       <c r="B117">
-        <v>-5.0651300000000003E-2</v>
+        <v>-1.76353E-2</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>0.11016280000000001</v>
+        <v>0.88983719999999999</v>
       </c>
       <c r="B118">
-        <v>-4.8456699999999998E-2</v>
+        <v>-1.5735099999999998E-2</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>9.5491500000000007E-2</v>
+        <v>0.90450850000000005</v>
       </c>
       <c r="B119">
-        <v>-4.6048899999999997E-2</v>
+        <v>-1.3914299999999999E-2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>8.1764900000000001E-2</v>
+        <v>0.91823509999999997</v>
       </c>
       <c r="B120">
-        <v>-4.3437099999999999E-2</v>
+        <v>-1.21823E-2</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>6.9015199999999999E-2</v>
+        <v>0.9309849</v>
       </c>
       <c r="B121">
-        <v>-4.0631E-2</v>
+        <v>-1.0548500000000001E-2</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>5.7272000000000003E-2</v>
+        <v>0.94272800000000001</v>
       </c>
       <c r="B122">
-        <v>-3.7641399999999998E-2</v>
+        <v>-9.0217000000000006E-3</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>4.6562800000000001E-2</v>
+        <v>0.95343719999999998</v>
       </c>
       <c r="B123">
-        <v>-3.4479200000000002E-2</v>
+        <v>-7.6108E-3</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>3.69127E-2</v>
+        <v>0.96308729999999998</v>
       </c>
       <c r="B124">
-        <v>-3.11559E-2</v>
+        <v>-6.3238000000000001E-3</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>2.8344100000000001E-2</v>
+        <v>0.97165590000000002</v>
       </c>
       <c r="B125">
-        <v>-2.7682700000000001E-2</v>
+        <v>-5.1685000000000004E-3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>2.0877099999999999E-2</v>
+        <v>0.97912290000000002</v>
       </c>
       <c r="B126">
-        <v>-2.4070600000000001E-2</v>
+        <v>-4.1519E-3</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>1.45291E-2</v>
+        <v>0.98547090000000004</v>
       </c>
       <c r="B127">
-        <v>-2.0330000000000001E-2</v>
+        <v>-3.2804000000000002E-3</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>9.3148999999999992E-3</v>
+        <v>0.99068500000000004</v>
       </c>
       <c r="B128">
-        <v>-1.6470599999999998E-2</v>
+        <v>-2.5595000000000001E-3</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>5.2468000000000002E-3</v>
+        <v>0.9947532</v>
       </c>
       <c r="B129">
-        <v>-1.2501099999999999E-2</v>
+        <v>-1.9938E-3</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>2.3341999999999998E-3</v>
+        <v>0.99766580000000005</v>
       </c>
       <c r="B130">
-        <v>-8.4288999999999996E-3</v>
+        <v>-1.5870000000000001E-3</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>5.8390000000000004E-4</v>
+        <v>0.99941610000000003</v>
       </c>
       <c r="B131">
-        <v>-4.2602999999999999E-3</v>
+        <v>-1.3419E-3</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>-1.2600000000000001E-3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A67:B132">
-    <sortCondition descending="1" ref="A67:A132"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A68:B131">
+    <sortCondition ref="A68:A131"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>